<commit_message>
update some ranges for new form input
**Final form will have columns g & h hidden in the form sheets**
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8292"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8292" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Initials" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,11 @@
     <sheet name="8PFormSheet" sheetId="3" r:id="rId3"/>
     <sheet name="3PFormSheet" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="Last_Row_Read_3P">'3PFormSheet'!$H$1</definedName>
+    <definedName name="Last_Row_Read_3W">'3WFormSheet'!$H$1</definedName>
+    <definedName name="Last_Row_Read_8P">'8PFormSheet'!$H$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="74">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -170,9 +175,6 @@
     <t>ST</t>
   </si>
   <si>
-    <t>ALW</t>
-  </si>
-  <si>
     <t>RZ</t>
   </si>
   <si>
@@ -204,6 +206,54 @@
   </si>
   <si>
     <t>KA</t>
+  </si>
+  <si>
+    <t>AWL</t>
+  </si>
+  <si>
+    <t>Last Row Read 8P:</t>
+  </si>
+  <si>
+    <t>Test Data:</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>4,5,6,7</t>
+  </si>
+  <si>
+    <t>wakka wakka</t>
+  </si>
+  <si>
+    <t>6,7,8</t>
+  </si>
+  <si>
+    <t>boom!</t>
+  </si>
+  <si>
+    <t>1,88,68</t>
+  </si>
+  <si>
+    <t>I am a sucka!</t>
+  </si>
+  <si>
+    <t>yaba dabba don't!</t>
+  </si>
+  <si>
+    <t>Last Row Read 3W:</t>
+  </si>
+  <si>
+    <t>Last Row Read 3P:</t>
   </si>
 </sst>
 </file>
@@ -306,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -441,12 +491,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -518,6 +605,27 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,7 +657,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1619250</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>73871</xdr:rowOff>
+      <xdr:rowOff>58631</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -665,7 +773,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1619250</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>73871</xdr:rowOff>
+      <xdr:rowOff>58631</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1010,7 +1118,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A144"/>
     </sheetView>
   </sheetViews>
@@ -1073,7 +1181,7 @@
     </row>
     <row r="12" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1303,12 +1411,12 @@
     </row>
     <row r="58" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="26" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1378,22 +1486,22 @@
     </row>
     <row r="73" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1438,22 +1546,22 @@
     </row>
     <row r="85" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1558,7 +1666,7 @@
     </row>
     <row r="109" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1618,7 +1726,7 @@
     </row>
     <row r="121" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1747,7 +1855,7 @@
   <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G1" sqref="G1:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1779,8 +1887,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="40">
+        <v>6</v>
+      </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -1867,11 +1979,13 @@
       <c r="D5" s="10"/>
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="G5" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -1889,11 +2003,19 @@
       <c r="D6" s="10"/>
       <c r="E6" s="12"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="G6" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="44"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -1904,18 +2026,26 @@
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="12"/>
       <c r="D7" s="10"/>
       <c r="E7" s="12"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="G7" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="45"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -1926,18 +2056,28 @@
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="12"/>
       <c r="D8" s="10"/>
       <c r="E8" s="12"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="G8" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>66</v>
+      </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -1955,11 +2095,21 @@
       <c r="D9" s="10"/>
       <c r="E9" s="12"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="G9" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>68</v>
+      </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
@@ -1970,18 +2120,28 @@
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="12"/>
       <c r="D10" s="10"/>
       <c r="E10" s="12"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="G10" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>70</v>
+      </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -1992,18 +2152,28 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="12"/>
       <c r="D11" s="10"/>
       <c r="E11" s="12"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="G11" s="7">
+        <v>43065</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="45" t="s">
+        <v>71</v>
+      </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
@@ -2763,6 +2933,9 @@
       <c r="Q53" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G5:K5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2775,7 +2948,7 @@
   <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="G1" sqref="G1:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2807,8 +2980,1161 @@
         <v>4</v>
       </c>
       <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="40">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>43064</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>43064</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>43064</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>43064</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>43064</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>43065</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="7">
+        <v>43065</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="5"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="5"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+    </row>
+    <row r="37" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+    </row>
+    <row r="38" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+    </row>
+    <row r="39" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+    </row>
+    <row r="40" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+    </row>
+    <row r="41" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="5"/>
+      <c r="S41" s="5"/>
+      <c r="T41" s="5"/>
+    </row>
+    <row r="42" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+    </row>
+    <row r="43" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="5"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="5"/>
+    </row>
+    <row r="44" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+    </row>
+    <row r="45" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+    </row>
+    <row r="46" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+    </row>
+    <row r="47" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+    </row>
+    <row r="48" spans="7:20" x14ac:dyDescent="0.3">
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+    </row>
+    <row r="51" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+    </row>
+    <row r="53" spans="7:17" x14ac:dyDescent="0.3">
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G5:K5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Rooms2"/>
+  <dimension ref="A1:T53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="16" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="6" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="40">
+        <v>6</v>
+      </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -2895,11 +4221,13 @@
       <c r="D5" s="10"/>
       <c r="E5" s="12"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="G5" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -2917,11 +4245,19 @@
       <c r="D6" s="10"/>
       <c r="E6" s="12"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="G6" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K6" s="44"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -2932,18 +4268,26 @@
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="12"/>
       <c r="D7" s="10"/>
       <c r="E7" s="12"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="G7" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="45"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -2954,18 +4298,28 @@
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="12"/>
       <c r="D8" s="10"/>
       <c r="E8" s="12"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="G8" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="45" t="s">
+        <v>66</v>
+      </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -2976,18 +4330,28 @@
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="12"/>
       <c r="D9" s="10"/>
       <c r="E9" s="12"/>
       <c r="F9" s="8"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="G9" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>68</v>
+      </c>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
@@ -2998,18 +4362,28 @@
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="12"/>
       <c r="D10" s="10"/>
       <c r="E10" s="12"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="G10" s="7">
+        <v>43064</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>70</v>
+      </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -3020,18 +4394,28 @@
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="12"/>
       <c r="D11" s="10"/>
       <c r="E11" s="12"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="G11" s="7">
+        <v>43065</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="45" t="s">
+        <v>71</v>
+      </c>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
@@ -3042,7 +4426,7 @@
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="12"/>
@@ -3791,1034 +5175,9 @@
       <c r="Q53" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Rooms2"/>
-  <dimension ref="A1:T53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.5546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="6" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
-      <c r="T13" s="5"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
-      <c r="T14" s="5"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
-      <c r="T17" s="5"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
-      <c r="T18" s="5"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="5"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
-      <c r="T22" s="5"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
-      <c r="T23" s="5"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-    </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-    </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
-      <c r="P34" s="5"/>
-      <c r="Q34" s="5"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
-    </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="5"/>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
-    </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
-      <c r="P36" s="5"/>
-      <c r="Q36" s="5"/>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
-    </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-    </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
-      <c r="P38" s="5"/>
-      <c r="Q38" s="5"/>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-    </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-    </row>
-    <row r="40" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
-      <c r="Q40" s="5"/>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
-    </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-    </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
-      <c r="P42" s="5"/>
-      <c r="Q42" s="5"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-    </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
-      <c r="P43" s="5"/>
-      <c r="Q43" s="5"/>
-      <c r="R43" s="5"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="5"/>
-    </row>
-    <row r="44" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
-      <c r="P44" s="5"/>
-      <c r="Q44" s="5"/>
-      <c r="R44" s="5"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="5"/>
-    </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="5"/>
-    </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5"/>
-      <c r="Q46" s="5"/>
-    </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="5"/>
-    </row>
-    <row r="48" spans="7:20" x14ac:dyDescent="0.3">
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5"/>
-      <c r="Q48" s="5"/>
-    </row>
-    <row r="49" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="5"/>
-    </row>
-    <row r="50" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
-      <c r="P50" s="5"/>
-      <c r="Q50" s="5"/>
-    </row>
-    <row r="51" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-      <c r="Q51" s="5"/>
-    </row>
-    <row r="52" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-      <c r="Q52" s="5"/>
-    </row>
-    <row r="53" spans="7:17" x14ac:dyDescent="0.3">
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
-      <c r="P53" s="5"/>
-      <c r="Q53" s="5"/>
-    </row>
-  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G5:K5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
updated to current forms
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="98">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -263,6 +263,69 @@
   </si>
   <si>
     <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</t>
+  </si>
+  <si>
+    <t>hot dog!</t>
+  </si>
+  <si>
+    <t>89,87</t>
+  </si>
+  <si>
+    <t>more testeroos</t>
+  </si>
+  <si>
+    <t>12,13</t>
+  </si>
+  <si>
+    <t>testing 1,2,3</t>
+  </si>
+  <si>
+    <t>hubba bubba</t>
+  </si>
+  <si>
+    <t>hoop</t>
+  </si>
+  <si>
+    <t>STUFF</t>
+  </si>
+  <si>
+    <t>stuff</t>
+  </si>
+  <si>
+    <t>i think it works</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>some more, one  last time</t>
+  </si>
+  <si>
+    <t>7,5,2</t>
+  </si>
+  <si>
+    <t>yabba dabba</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>whatcha doin?</t>
+  </si>
+  <si>
+    <t>hubba</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>erd</t>
+  </si>
+  <si>
+    <t>goop</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
 </sst>
 </file>
@@ -639,7 +702,7 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -713,6 +776,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -728,14 +798,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1247,7 +1316,7 @@
   <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,13 +1339,13 @@
       <c r="D2" s="38">
         <v>0</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
@@ -1288,13 +1357,13 @@
       <c r="D3" s="38">
         <v>0</v>
       </c>
-      <c r="E3" s="44" t="s">
+      <c r="E3" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
@@ -1306,13 +1375,13 @@
       <c r="D4" s="38">
         <v>0</v>
       </c>
-      <c r="E4" s="49" t="s">
+      <c r="E4" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
@@ -1323,13 +1392,13 @@
       <c r="A6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="46"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
@@ -1347,7 +1416,7 @@
       <c r="F7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="39"/>
+      <c r="G7" s="40"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
@@ -1365,7 +1434,7 @@
       <c r="F8" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="40"/>
+      <c r="G8" s="41"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
@@ -1383,7 +1452,7 @@
       <c r="F9" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="41" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1403,7 +1472,7 @@
       <c r="F10" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="40" t="s">
+      <c r="G10" s="41" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1423,7 +1492,7 @@
       <c r="F11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="40" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1443,7 +1512,7 @@
       <c r="F12" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="41" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2124,7 +2193,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2158,67 +2227,147 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="10"/>
+      <c r="A3" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="10"/>
+      <c r="A4" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>93</v>
+      </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>94</v>
+      </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="10"/>
+      <c r="A6" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="10"/>
+      <c r="A7" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="8">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="10"/>
+      <c r="A8" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>96</v>
+      </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="10"/>
+      <c r="A9" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2381,10 +2530,452 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Rooms"/>
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="17" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5">
+        <v>43064</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="42"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>43064</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="43"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>43064</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>43064</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>43064</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="8">
+        <v>4</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="8">
+        <v>7</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="8">
+        <v>9</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="15"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="15"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="15"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E41" s="15"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="15"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E43" s="15"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="15"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="15"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="15"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="15"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="15"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="15"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Rooms2"/>
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E7"/>
+      <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2419,109 +3010,101 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>43064</v>
+        <v>43065</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="39"/>
+        <v>20</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>43064</v>
+        <v>43065</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>63</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="40"/>
+        <v>78</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>43064</v>
+        <v>43065</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="40" t="s">
-        <v>66</v>
+        <v>80</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>43064</v>
+        <v>43065</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="8">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>43065</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>43064</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>70</v>
+      <c r="D6" s="8">
+        <v>6</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>43065</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>71</v>
-      </c>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="10"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="10"/>
@@ -2529,7 +3112,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
@@ -2537,7 +3120,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
@@ -2545,7 +3128,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="10"/>
@@ -2553,7 +3136,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="10"/>
@@ -2692,264 +3275,4 @@
   <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Rooms2"/>
-  <dimension ref="A1:F28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.5546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
make communicator match uploaded files
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8292"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8292" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Initials" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="3PFormSheet" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="All_Initials">Initials!$A$1:$A$144</definedName>
     <definedName name="Last_Row_Read_3P">Initials!$D$4</definedName>
     <definedName name="Last_Row_Read_3W">Initials!$D$2</definedName>
     <definedName name="Last_Row_Read_8P">Initials!$D$3</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="91">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -49,6 +50,78 @@
     <t>Comments</t>
   </si>
   <si>
+    <t>KX</t>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>JW</t>
+  </si>
+  <si>
+    <t>Last Row Read 8P:</t>
+  </si>
+  <si>
+    <t>Test Data:</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>4,5,6,7</t>
+  </si>
+  <si>
+    <t>wakka wakka</t>
+  </si>
+  <si>
+    <t>6,7,8</t>
+  </si>
+  <si>
+    <t>boom!</t>
+  </si>
+  <si>
+    <t>1,88,68</t>
+  </si>
+  <si>
+    <t>I am a sucka!</t>
+  </si>
+  <si>
+    <t>yaba dabba don't!</t>
+  </si>
+  <si>
+    <t>Last Row Read 3W:</t>
+  </si>
+  <si>
+    <t>Last Row Read 3P:</t>
+  </si>
+  <si>
+    <t>0 = not cleared</t>
+  </si>
+  <si>
+    <t>1 = cleared</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</t>
+  </si>
+  <si>
     <t>CW</t>
   </si>
   <si>
@@ -58,9 +131,6 @@
     <t>EC</t>
   </si>
   <si>
-    <t>KX</t>
-  </si>
-  <si>
     <t>ABB</t>
   </si>
   <si>
@@ -82,36 +152,27 @@
     <t>MK</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>DG</t>
+  </si>
+  <si>
     <t>VR</t>
   </si>
   <si>
-    <t>MW</t>
-  </si>
-  <si>
-    <t>GB</t>
-  </si>
-  <si>
-    <t>KC</t>
-  </si>
-  <si>
-    <t>KH</t>
-  </si>
-  <si>
-    <t>DG</t>
-  </si>
-  <si>
-    <t>RM</t>
-  </si>
-  <si>
     <t>JS</t>
   </si>
   <si>
-    <t>KS</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>KL</t>
   </si>
   <si>
@@ -154,15 +215,9 @@
     <t>LG</t>
   </si>
   <si>
-    <t>AB</t>
-  </si>
-  <si>
     <t>KGH</t>
   </si>
   <si>
-    <t>JW</t>
-  </si>
-  <si>
     <t>LF</t>
   </si>
   <si>
@@ -175,6 +230,9 @@
     <t>ST</t>
   </si>
   <si>
+    <t>AWL</t>
+  </si>
+  <si>
     <t>RZ</t>
   </si>
   <si>
@@ -208,61 +266,25 @@
     <t>KA</t>
   </si>
   <si>
-    <t>AWL</t>
-  </si>
-  <si>
-    <t>Last Row Read 8P:</t>
-  </si>
-  <si>
-    <t>Test Data:</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>1,2,3</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>1,2,3,4</t>
-  </si>
-  <si>
-    <t>4,5,6,7</t>
-  </si>
-  <si>
-    <t>wakka wakka</t>
-  </si>
-  <si>
-    <t>6,7,8</t>
-  </si>
-  <si>
-    <t>boom!</t>
-  </si>
-  <si>
-    <t>1,88,68</t>
-  </si>
-  <si>
-    <t>I am a sucka!</t>
-  </si>
-  <si>
-    <t>yaba dabba don't!</t>
-  </si>
-  <si>
-    <t>Last Row Read 3W:</t>
-  </si>
-  <si>
-    <t>Last Row Read 3P:</t>
-  </si>
-  <si>
-    <t>0 = not cleared</t>
-  </si>
-  <si>
-    <t>1 = cleared</t>
-  </si>
-  <si>
-    <t>&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;&lt;</t>
+    <t>hoop dreams!</t>
+  </si>
+  <si>
+    <t>STUFF</t>
+  </si>
+  <si>
+    <t>stuff</t>
+  </si>
+  <si>
+    <t>i think it works</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>some more, one  last time</t>
+  </si>
+  <si>
+    <t>comments</t>
   </si>
   <si>
     <t>hot dog!</t>
@@ -283,49 +305,7 @@
     <t>hubba bubba</t>
   </si>
   <si>
-    <t>hoop</t>
-  </si>
-  <si>
-    <t>STUFF</t>
-  </si>
-  <si>
-    <t>stuff</t>
-  </si>
-  <si>
-    <t>i think it works</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>some more, one  last time</t>
-  </si>
-  <si>
-    <t>7,5,2</t>
-  </si>
-  <si>
-    <t>yabba dabba</t>
-  </si>
-  <si>
-    <t>ER</t>
-  </si>
-  <si>
-    <t>whatcha doin?</t>
-  </si>
-  <si>
-    <t>hubba</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>erd</t>
-  </si>
-  <si>
-    <t>goop</t>
-  </si>
-  <si>
-    <t>comments</t>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -397,30 +377,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF5050"/>
-        <bgColor rgb="FFFF5050"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF00B0F0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA570C6"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -455,6 +411,30 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5050"/>
+        <bgColor rgb="FFFF5050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FF00B0F0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA570C6"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -474,6 +454,105 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -591,115 +670,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="53">
@@ -751,29 +731,10 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -789,31 +750,50 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1315,7 +1295,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1325,75 +1305,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="19">
+        <v>0</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="48"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="19">
+        <v>0</v>
+      </c>
+      <c r="E3" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="50"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="D2" s="38">
+      <c r="C4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="19">
         <v>0</v>
       </c>
-      <c r="E2" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="48"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="38">
-        <v>0</v>
-      </c>
-      <c r="E3" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="50"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="38">
-        <v>0</v>
-      </c>
       <c r="E4" s="51" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="F4" s="52"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
-        <v>9</v>
+      <c r="A5" s="25" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
-        <v>10</v>
+      <c r="A6" s="25" t="s">
+        <v>33</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="D6" s="45"/>
       <c r="E6" s="45"/>
@@ -1401,779 +1381,779 @@
       <c r="G6" s="46"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>11</v>
+      <c r="A7" s="25" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="5">
         <v>43064</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="40"/>
+        <v>14</v>
+      </c>
+      <c r="G7" s="21"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
-        <v>12</v>
+      <c r="A8" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="5">
         <v>43064</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="41"/>
+        <v>16</v>
+      </c>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>13</v>
+      <c r="A9" s="25" t="s">
+        <v>36</v>
       </c>
       <c r="C9" s="5">
         <v>43064</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>66</v>
+        <v>17</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
-        <v>14</v>
+      <c r="A10" s="25" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="5">
         <v>43064</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="41" t="s">
-        <v>68</v>
+        <v>19</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
-        <v>15</v>
+      <c r="A11" s="25" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="5">
         <v>43064</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
-        <v>25</v>
+      <c r="A12" s="26" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="5">
         <v>43065</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="32" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="8" t="s">
+    </row>
+    <row r="55" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="41" t="s">
+    </row>
+    <row r="56" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A79" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="33" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="24" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="24" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="24" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="24" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A55" s="24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A56" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A57" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A58" s="24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A59" s="24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A61" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A62" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A64" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A65" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A68" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A73" s="26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A78" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A81" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A83" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="26" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="86" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="27" t="s">
-        <v>53</v>
+      <c r="A86" s="34" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A87" s="27" t="s">
-        <v>54</v>
+      <c r="A87" s="34" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A88" s="27" t="s">
-        <v>55</v>
+      <c r="A88" s="34" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A89" s="27" t="s">
-        <v>25</v>
+      <c r="A89" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A90" s="27" t="s">
-        <v>25</v>
+      <c r="A90" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A91" s="27" t="s">
-        <v>25</v>
+      <c r="A91" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="27" t="s">
-        <v>25</v>
+      <c r="A92" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="27" t="s">
-        <v>25</v>
+      <c r="A93" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="27" t="s">
-        <v>25</v>
+      <c r="A94" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="27" t="s">
-        <v>25</v>
+      <c r="A95" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="28" t="s">
-        <v>25</v>
+      <c r="A96" s="35" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="29" t="s">
-        <v>25</v>
+      <c r="A97" s="36" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="30" t="s">
-        <v>25</v>
+      <c r="A98" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="30" t="s">
-        <v>25</v>
+      <c r="A99" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="30" t="s">
-        <v>25</v>
+      <c r="A100" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="30" t="s">
-        <v>25</v>
+      <c r="A101" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A102" s="30" t="s">
-        <v>25</v>
+      <c r="A102" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A103" s="30" t="s">
-        <v>25</v>
+      <c r="A103" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="30" t="s">
-        <v>25</v>
+      <c r="A104" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A105" s="30" t="s">
-        <v>25</v>
+      <c r="A105" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="30" t="s">
-        <v>25</v>
+      <c r="A106" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A107" s="30" t="s">
-        <v>25</v>
+      <c r="A107" s="37" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="31" t="s">
-        <v>25</v>
+      <c r="A108" s="38" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A109" s="32" t="s">
-        <v>56</v>
+      <c r="A109" s="39" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A110" s="33" t="s">
-        <v>25</v>
+      <c r="A110" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A111" s="33" t="s">
-        <v>25</v>
+      <c r="A111" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A112" s="33" t="s">
-        <v>25</v>
+      <c r="A112" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A113" s="33" t="s">
-        <v>25</v>
+      <c r="A113" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A114" s="33" t="s">
-        <v>25</v>
+      <c r="A114" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A115" s="33" t="s">
-        <v>25</v>
+      <c r="A115" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="33" t="s">
-        <v>25</v>
+      <c r="A116" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="33" t="s">
-        <v>25</v>
+      <c r="A117" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A118" s="33" t="s">
-        <v>25</v>
+      <c r="A118" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="33" t="s">
-        <v>25</v>
+      <c r="A119" s="40" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="34" t="s">
-        <v>25</v>
+      <c r="A120" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A121" s="35" t="s">
-        <v>57</v>
+      <c r="A121" s="42" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A122" s="34" t="s">
-        <v>25</v>
+      <c r="A122" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A123" s="34" t="s">
-        <v>25</v>
+      <c r="A123" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A124" s="34" t="s">
-        <v>25</v>
+      <c r="A124" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="34" t="s">
-        <v>25</v>
+      <c r="A125" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="34" t="s">
-        <v>25</v>
+      <c r="A126" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A127" s="34" t="s">
-        <v>25</v>
+      <c r="A127" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A128" s="34" t="s">
-        <v>25</v>
+      <c r="A128" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A129" s="34" t="s">
-        <v>25</v>
+      <c r="A129" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A130" s="34" t="s">
-        <v>25</v>
+      <c r="A130" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A131" s="34" t="s">
-        <v>25</v>
+      <c r="A131" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="34" t="s">
-        <v>25</v>
+      <c r="A132" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A133" s="35" t="s">
-        <v>25</v>
+      <c r="A133" s="42" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A134" s="34" t="s">
-        <v>25</v>
+      <c r="A134" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A135" s="34" t="s">
-        <v>25</v>
+      <c r="A135" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A136" s="34" t="s">
-        <v>25</v>
+      <c r="A136" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A137" s="34" t="s">
-        <v>25</v>
+      <c r="A137" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A138" s="34" t="s">
-        <v>25</v>
+      <c r="A138" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A139" s="34" t="s">
-        <v>25</v>
+      <c r="A139" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A140" s="34" t="s">
-        <v>25</v>
+      <c r="A140" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A141" s="34" t="s">
-        <v>25</v>
+      <c r="A141" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A142" s="34" t="s">
-        <v>25</v>
+      <c r="A142" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A143" s="34" t="s">
-        <v>25</v>
+      <c r="A143" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A144" s="36" t="s">
-        <v>25</v>
+      <c r="A144" s="43" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2192,7 +2172,7 @@
   <sheetPr codeName="Rooms1"/>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
@@ -2228,91 +2208,87 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>43065</v>
+        <v>43064</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>90</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E2" s="23"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>43065</v>
+        <v>43064</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>91</v>
+        <v>9</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>92</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="24"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>43065</v>
+        <v>43064</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>93</v>
+        <v>15</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>43065</v>
+        <v>43064</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>94</v>
+        <v>13</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>43065</v>
+        <v>43064</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="8">
-        <v>2</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>85</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>22</v>
       </c>
       <c r="F6" s="6"/>
     </row>
@@ -2321,16 +2297,16 @@
         <v>43065</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>95</v>
       </c>
       <c r="F7" s="6"/>
     </row>
@@ -2339,35 +2315,25 @@
         <v>43065</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="D8" s="8">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>43065</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="8">
-        <v>2</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>97</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2571,15 +2537,15 @@
         <v>43064</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="42"/>
+        <v>14</v>
+      </c>
+      <c r="E2" s="23"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -2587,15 +2553,15 @@
         <v>43064</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="43"/>
+        <v>16</v>
+      </c>
+      <c r="E3" s="24"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -2603,16 +2569,16 @@
         <v>43064</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>66</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -2621,16 +2587,16 @@
         <v>43064</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>68</v>
+        <v>19</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>20</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -2639,16 +2605,16 @@
         <v>43064</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>22</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>70</v>
       </c>
       <c r="F6" s="6"/>
     </row>
@@ -2657,16 +2623,16 @@
         <v>43065</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="43" t="s">
-        <v>71</v>
+        <v>14</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="F7" s="6"/>
     </row>
@@ -2675,16 +2641,16 @@
         <v>43066</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D8" s="8">
         <v>2</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F8" s="6"/>
     </row>
@@ -2693,16 +2659,16 @@
         <v>43066</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F9" s="6"/>
     </row>
@@ -2711,16 +2677,16 @@
         <v>43066</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D10" s="8">
         <v>4</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F10" s="6"/>
     </row>
@@ -2729,16 +2695,16 @@
         <v>43066</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D11" s="8">
         <v>7</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F11" s="6"/>
     </row>
@@ -2747,16 +2713,16 @@
         <v>43066</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F12" s="6"/>
     </row>
@@ -2765,16 +2731,16 @@
         <v>43066</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="8">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F13" s="6"/>
     </row>
@@ -3013,14 +2979,14 @@
         <v>43065</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8">
         <v>1</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -3029,16 +2995,16 @@
         <v>43065</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -3047,16 +3013,16 @@
         <v>43065</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -3065,16 +3031,16 @@
         <v>43065</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D5" s="8">
         <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="F5" s="6"/>
     </row>
@@ -3083,16 +3049,16 @@
         <v>43065</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="D6" s="8">
         <v>6</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="F6" s="6"/>
     </row>

</xml_diff>

<commit_message>
yes and no call offs importing into all therapists; groups highlighting in all schedules and ind schedules
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\trident tech\IST 286 Internship\Schedule Versions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\Roper\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8292" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8295" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initials" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="Last_Row_Read_3W">Initials!$D$2</definedName>
     <definedName name="Last_Row_Read_8P">Initials!$D$3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="92">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -306,12 +306,15 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>92A, 881</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
@@ -798,15 +801,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="20% - Accent1 2" xfId="2"/>
-    <cellStyle name="20% - Accent2 2" xfId="4"/>
-    <cellStyle name="20% - Accent6 2" xfId="6"/>
-    <cellStyle name="40% - Accent1 2" xfId="3"/>
-    <cellStyle name="40% - Accent2 2" xfId="5"/>
-    <cellStyle name="40% - Accent6 2" xfId="7"/>
+    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 21 2" xfId="1"/>
-    <cellStyle name="Normal 4 2" xfId="8"/>
+    <cellStyle name="Normal 21 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 4 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1291,7 +1294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I144"/>
   <sheetViews>
@@ -1299,17 +1302,17 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>30</v>
       </c>
@@ -1327,7 +1330,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>31</v>
       </c>
@@ -1345,7 +1348,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>5</v>
       </c>
@@ -1363,12 +1366,12 @@
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>33</v>
       </c>
@@ -1380,7 +1383,7 @@
       <c r="F6" s="45"/>
       <c r="G6" s="46"/>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>34</v>
       </c>
@@ -1398,7 +1401,7 @@
       </c>
       <c r="G7" s="21"/>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>35</v>
       </c>
@@ -1416,7 +1419,7 @@
       </c>
       <c r="G8" s="22"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>36</v>
       </c>
@@ -1436,7 +1439,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>37</v>
       </c>
@@ -1456,7 +1459,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>38</v>
       </c>
@@ -1476,7 +1479,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>39</v>
       </c>
@@ -1496,662 +1499,662 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="31" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="31" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="32" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="33" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="34" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="33" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="34" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="37" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="39" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="130" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="43" t="s">
         <v>39</v>
       </c>
@@ -2168,27 +2171,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Rooms1"/>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="16.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2206,7 +2209,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43064</v>
       </c>
@@ -2222,7 +2225,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43064</v>
       </c>
@@ -2238,7 +2241,7 @@
       <c r="E3" s="24"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43064</v>
       </c>
@@ -2256,7 +2259,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43064</v>
       </c>
@@ -2274,7 +2277,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43064</v>
       </c>
@@ -2292,7 +2295,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43065</v>
       </c>
@@ -2310,7 +2313,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43065</v>
       </c>
@@ -2328,7 +2331,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
@@ -2336,7 +2339,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
@@ -2344,7 +2347,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="10"/>
@@ -2352,7 +2355,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="10"/>
@@ -2360,7 +2363,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="10"/>
@@ -2368,7 +2371,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="10"/>
@@ -2376,7 +2379,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="10"/>
@@ -2384,7 +2387,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
@@ -2392,7 +2395,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="10"/>
@@ -2400,7 +2403,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="10"/>
@@ -2408,7 +2411,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="10"/>
@@ -2416,7 +2419,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="10"/>
@@ -2424,7 +2427,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="10"/>
@@ -2432,7 +2435,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="10"/>
@@ -2440,7 +2443,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="10"/>
@@ -2448,7 +2451,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="10"/>
@@ -2456,7 +2459,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="10"/>
@@ -2464,7 +2467,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="10"/>
@@ -2472,7 +2475,7 @@
       <c r="E26" s="10"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
@@ -2480,7 +2483,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="D28" s="11"/>
       <c r="E28" s="10"/>
@@ -2494,27 +2497,27 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Rooms"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="16.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2532,7 +2535,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43064</v>
       </c>
@@ -2548,7 +2551,7 @@
       <c r="E2" s="23"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43064</v>
       </c>
@@ -2564,7 +2567,7 @@
       <c r="E3" s="24"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43064</v>
       </c>
@@ -2582,7 +2585,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43064</v>
       </c>
@@ -2600,7 +2603,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43064</v>
       </c>
@@ -2618,7 +2621,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43065</v>
       </c>
@@ -2636,7 +2639,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43066</v>
       </c>
@@ -2654,7 +2657,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43066</v>
       </c>
@@ -2672,7 +2675,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43066</v>
       </c>
@@ -2690,7 +2693,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43066</v>
       </c>
@@ -2708,7 +2711,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>43066</v>
       </c>
@@ -2726,7 +2729,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>43066</v>
       </c>
@@ -2736,23 +2739,31 @@
       <c r="C13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>14</v>
+      <c r="D13" s="8">
+        <v>9</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>83</v>
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="8"/>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="10"/>
@@ -2760,7 +2771,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
@@ -2768,7 +2779,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="10"/>
@@ -2776,7 +2787,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="10"/>
@@ -2784,7 +2795,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="10"/>
@@ -2792,7 +2803,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="10"/>
@@ -2800,7 +2811,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="10"/>
@@ -2808,7 +2819,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="10"/>
@@ -2816,7 +2827,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="10"/>
@@ -2824,7 +2835,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="10"/>
@@ -2832,7 +2843,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="10"/>
@@ -2840,7 +2851,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="10"/>
@@ -2848,7 +2859,7 @@
       <c r="E26" s="10"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
@@ -2856,76 +2867,76 @@
       <c r="E27" s="10"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="D28" s="11"/>
       <c r="E28" s="10"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="15"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" s="15"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" s="15"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E40" s="15"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E41" s="15"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E42" s="15"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E43" s="15"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E44" s="15"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E45" s="15"/>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E46" s="15"/>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E47" s="15"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E48" s="15"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E49" s="15"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E50" s="15"/>
     </row>
   </sheetData>
@@ -2936,7 +2947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Rooms2"/>
   <dimension ref="A1:F28"/>
   <sheetViews>
@@ -2944,19 +2955,19 @@
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="27.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.5546875" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="16.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="42.7109375" style="15" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2974,7 +2985,7 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>43065</v>
       </c>
@@ -2990,7 +3001,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>43065</v>
       </c>
@@ -3008,7 +3019,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>43065</v>
       </c>
@@ -3026,7 +3037,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43065</v>
       </c>
@@ -3044,7 +3055,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43065</v>
       </c>
@@ -3062,7 +3073,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="10"/>
@@ -3070,7 +3081,7 @@
       <c r="E7" s="10"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="10"/>
@@ -3078,7 +3089,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
@@ -3086,7 +3097,7 @@
       <c r="E9" s="10"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
@@ -3094,7 +3105,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="10"/>
@@ -3102,7 +3113,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="10"/>
@@ -3110,7 +3121,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="10"/>
@@ -3118,7 +3129,7 @@
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="10"/>
@@ -3126,7 +3137,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="10"/>
@@ -3134,7 +3145,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
@@ -3142,7 +3153,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="10"/>
@@ -3150,7 +3161,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="10"/>
@@ -3158,7 +3169,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="10"/>
@@ -3166,7 +3177,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="10"/>
@@ -3174,7 +3185,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="10"/>
@@ -3182,7 +3193,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="10"/>
@@ -3190,7 +3201,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="10"/>
@@ -3198,7 +3209,7 @@
       <c r="E23" s="10"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="10"/>
@@ -3206,7 +3217,7 @@
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="10"/>
@@ -3214,7 +3225,7 @@
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="10"/>
@@ -3222,7 +3233,7 @@
       <c r="E26" s="10"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
@@ -3230,7 +3241,7 @@
       <c r="E27" s="10"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="D28" s="11"/>
       <c r="E28" s="10"/>

</xml_diff>

<commit_message>
added check to see if file exists before calling IsFileOpen in therapist forms to eliminate an error the first time the calls are made.
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8295" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initials" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="86">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -285,24 +285,6 @@
   </si>
   <si>
     <t>comments</t>
-  </si>
-  <si>
-    <t>hot dog!</t>
-  </si>
-  <si>
-    <t>89,87</t>
-  </si>
-  <si>
-    <t>more testeroos</t>
-  </si>
-  <si>
-    <t>12,13</t>
-  </si>
-  <si>
-    <t>testing 1,2,3</t>
-  </si>
-  <si>
-    <t>hubba bubba</t>
   </si>
   <si>
     <t>No</t>
@@ -1356,7 +1338,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>28</v>
@@ -2321,7 +2303,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D8" s="8">
         <v>42</v>
@@ -2501,7 +2483,7 @@
   <sheetPr codeName="Rooms"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
@@ -2758,7 +2740,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="6"/>
@@ -2951,7 +2933,7 @@
   <sheetPr codeName="Rooms2"/>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
@@ -2986,91 +2968,43 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>43065</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="8">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>84</v>
-      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>43065</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>86</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>43065</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>88</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>43065</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>89</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>43065</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="8">
-        <v>6</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>83</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add more rooms seems to be working now
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8295" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initials" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="92">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -266,31 +266,49 @@
     <t>KA</t>
   </si>
   <si>
-    <t>hoop dreams!</t>
-  </si>
-  <si>
-    <t>STUFF</t>
-  </si>
-  <si>
-    <t>stuff</t>
-  </si>
-  <si>
-    <t>i think it works</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>some more, one  last time</t>
-  </si>
-  <si>
-    <t>comments</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>NO COMMENT</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>92A, 881</t>
+    <t>7,8</t>
+  </si>
+  <si>
+    <t>12,13</t>
+  </si>
+  <si>
+    <t>9,11</t>
+  </si>
+  <si>
+    <t>83,84</t>
+  </si>
+  <si>
+    <t>NOT A COMMENT</t>
+  </si>
+  <si>
+    <t>90A,92B</t>
+  </si>
+  <si>
+    <t>883,92A</t>
+  </si>
+  <si>
+    <t>91A,98B</t>
+  </si>
+  <si>
+    <t>880, 881</t>
+  </si>
+  <si>
+    <t>882, 886</t>
+  </si>
+  <si>
+    <t>882,886</t>
   </si>
 </sst>
 </file>
@@ -667,7 +685,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -780,6 +798,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1338,7 +1359,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="51" t="s">
         <v>28</v>
@@ -2193,147 +2214,161 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43064</v>
+        <v>43066</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="23"/>
+        <v>78</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>79</v>
+      </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43064</v>
+        <v>43066</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43064</v>
+        <v>43066</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C4" s="10"/>
       <c r="D4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>18</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="E4" s="24"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>43064</v>
+        <v>43066</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>13</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C5" s="10"/>
       <c r="D5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>20</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="E5" s="24"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43064</v>
+        <v>43066</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>22</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E6" s="23"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>43065</v>
+        <v>43066</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>23</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E7" s="24"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>43065</v>
+        <v>43066</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="8">
-        <v>42</v>
-      </c>
-      <c r="E8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="8"/>
       <c r="E9" s="10"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="8"/>
+      <c r="A11" s="5">
+        <v>43066</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>84</v>
+      </c>
       <c r="E11" s="10"/>
       <c r="F11" s="6"/>
     </row>
@@ -2483,7 +2518,7 @@
   <sheetPr codeName="Rooms"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
@@ -2519,214 +2554,188 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>43064</v>
+        <v>43067</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="23"/>
+      <c r="D2" s="10">
+        <v>880881</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>85</v>
+      </c>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <v>43064</v>
+        <v>43067</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>16</v>
+      <c r="D3" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>43064</v>
+        <v>43067</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>18</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="24"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>43064</v>
+        <v>43067</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>20</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="24"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>43064</v>
+        <v>43067</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>22</v>
-      </c>
+      <c r="D6" s="10">
+        <v>882886</v>
+      </c>
+      <c r="E6" s="23"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>43065</v>
+        <v>43067</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="D7" s="10">
+        <v>880881</v>
+      </c>
+      <c r="E7" s="24"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>43066</v>
+        <v>43067</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="8">
-        <v>2</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>77</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="10"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>43066</v>
+        <v>43067</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>78</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>43066</v>
+        <v>43067</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="8">
-        <v>4</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>79</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="10"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>43066</v>
+        <v>43067</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="8">
-        <v>7</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>80</v>
-      </c>
+      <c r="D11" s="10">
+        <v>882886</v>
+      </c>
+      <c r="E11" s="10"/>
       <c r="F11" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>43066</v>
+        <v>43067</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>82</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10">
+        <v>880881</v>
+      </c>
+      <c r="E12" s="10"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>43066</v>
+        <v>43067</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="8">
-        <v>9</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>83</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10">
+        <v>880881</v>
+      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2734,191 +2743,300 @@
         <v>43067</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>85</v>
+        <v>40</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10">
+        <v>880881</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="10">
+        <v>882886</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="8"/>
+      <c r="D16" s="10">
+        <v>882886</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="8"/>
+      <c r="D17" s="10">
+        <v>880881</v>
+      </c>
       <c r="E17" s="10"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
+      <c r="D18" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="E18" s="10"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="C19" s="10"/>
-      <c r="D19" s="8"/>
+      <c r="D19" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>40</v>
+      </c>
       <c r="C20" s="10"/>
-      <c r="D20" s="8"/>
+      <c r="D20" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="10">
+        <v>882886</v>
+      </c>
       <c r="E21" s="10"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C22" s="10"/>
-      <c r="D22" s="8"/>
+      <c r="D22" s="10" t="s">
+        <v>90</v>
+      </c>
       <c r="E22" s="10"/>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C23" s="10"/>
-      <c r="D23" s="8"/>
+      <c r="D23" s="10">
+        <v>882886</v>
+      </c>
       <c r="E23" s="10"/>
       <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C24" s="10"/>
-      <c r="D24" s="8"/>
+      <c r="D24" s="10">
+        <v>882886</v>
+      </c>
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C25" s="10"/>
-      <c r="D25" s="8"/>
+      <c r="D25" s="10">
+        <v>882886</v>
+      </c>
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="10"/>
+      <c r="D26" s="53">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="11"/>
+      <c r="D27" s="53">
+        <v>882886</v>
+      </c>
       <c r="E27" s="10"/>
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="5"/>
-      <c r="D28" s="11"/>
+      <c r="A28" s="5">
+        <v>43067</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>91</v>
+      </c>
       <c r="E28" s="10"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="15"/>
       <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="15"/>
       <c r="E30" s="15"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="15"/>
       <c r="E31" s="15"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="15"/>
       <c r="E32" s="15"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="15"/>
       <c r="E33" s="15"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="15"/>
       <c r="E34" s="15"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="15"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="15"/>
       <c r="E36" s="15"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="15"/>
       <c r="E37" s="15"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="15"/>
       <c r="E38" s="15"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D39" s="15"/>
       <c r="E39" s="15"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D40" s="15"/>
       <c r="E40" s="15"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="15"/>
       <c r="E41" s="15"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="15"/>
       <c r="E42" s="15"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="15"/>
       <c r="E43" s="15"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="15"/>
       <c r="E44" s="15"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D45" s="15"/>
       <c r="E45" s="15"/>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D46" s="15"/>
       <c r="E46" s="15"/>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D47" s="15"/>
       <c r="E47" s="15"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="15"/>
       <c r="E48" s="15"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="15"/>
       <c r="E49" s="15"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="15"/>
       <c r="E50" s="15"/>
     </row>
   </sheetData>
@@ -2933,7 +3051,7 @@
   <sheetPr codeName="Rooms2"/>
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tweaked diddie formatting; added dummy data; everything seems to work
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="93">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -309,6 +309,9 @@
   </si>
   <si>
     <t>882,886</t>
+  </si>
+  <si>
+    <t>880,881</t>
   </si>
 </sst>
 </file>
@@ -772,6 +775,9 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -798,9 +804,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1325,10 +1328,10 @@
       <c r="D2" s="19">
         <v>0</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="48"/>
+      <c r="F2" s="49"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -1343,10 +1346,10 @@
       <c r="D3" s="19">
         <v>0</v>
       </c>
-      <c r="E3" s="49" t="s">
+      <c r="E3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="50"/>
+      <c r="F3" s="51"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -1361,10 +1364,10 @@
       <c r="D4" s="19">
         <v>0</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="52"/>
+      <c r="F4" s="53"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -1378,13 +1381,13 @@
       <c r="A6" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
@@ -2916,7 +2919,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="53">
+      <c r="D26" s="44">
         <v>0</v>
       </c>
       <c r="E26" s="10" t="s">
@@ -2932,7 +2935,7 @@
         <v>43</v>
       </c>
       <c r="C27" s="13"/>
-      <c r="D27" s="53">
+      <c r="D27" s="44">
         <v>882886</v>
       </c>
       <c r="E27" s="10"/>
@@ -2945,14 +2948,22 @@
       <c r="B28" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="53" t="s">
+      <c r="D28" s="44" t="s">
         <v>91</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D29" s="15"/>
+      <c r="A29" s="16">
+        <v>43067</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="E29" s="15"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
clearing yes and no columns and not allowing yes and
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8295" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8295" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Initials" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="85">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -264,30 +264,6 @@
   </si>
   <si>
     <t>KA</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>2,3</t>
-  </si>
-  <si>
-    <t>NO COMMENT</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>7,8</t>
-  </si>
-  <si>
-    <t>12,13</t>
-  </si>
-  <si>
-    <t>9,11</t>
-  </si>
-  <si>
-    <t>83,84</t>
   </si>
   <si>
     <t>NOT A COMMENT</t>
@@ -2179,9 +2155,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Rooms1"/>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
@@ -2216,162 +2192,82 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>79</v>
-      </c>
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="23"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>81</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="24"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="10"/>
-      <c r="D4" s="8" t="s">
-        <v>82</v>
-      </c>
+      <c r="D4" s="10"/>
       <c r="E4" s="24"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="8" t="s">
-        <v>83</v>
-      </c>
+      <c r="D5" s="10"/>
       <c r="E5" s="24"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="23"/>
       <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>78</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="24"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>81</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>83</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>79</v>
-      </c>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>43066</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>84</v>
-      </c>
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="6"/>
     </row>
@@ -2379,7 +2275,7 @@
       <c r="A12" s="5"/>
       <c r="B12" s="6"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="8"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="6"/>
     </row>
@@ -2387,7 +2283,7 @@
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="10"/>
-      <c r="D13" s="8"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="6"/>
     </row>
@@ -2395,7 +2291,7 @@
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="10"/>
-      <c r="D14" s="8"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="6"/>
     </row>
@@ -2403,7 +2299,7 @@
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="10"/>
-      <c r="D15" s="8"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="6"/>
     </row>
@@ -2411,7 +2307,7 @@
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="8"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="6"/>
     </row>
@@ -2419,7 +2315,7 @@
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="8"/>
+      <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="6"/>
     </row>
@@ -2427,7 +2323,7 @@
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="6"/>
     </row>
@@ -2435,7 +2331,7 @@
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="8"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
     </row>
@@ -2443,7 +2339,7 @@
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="10"/>
-      <c r="D20" s="8"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
     </row>
@@ -2451,7 +2347,7 @@
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="10"/>
-      <c r="D21" s="8"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="6"/>
     </row>
@@ -2459,7 +2355,7 @@
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="8"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="6"/>
     </row>
@@ -2467,7 +2363,7 @@
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="8"/>
+      <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="6"/>
     </row>
@@ -2475,7 +2371,7 @@
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="10"/>
-      <c r="D24" s="8"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="6"/>
     </row>
@@ -2483,7 +2379,7 @@
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="10"/>
-      <c r="D25" s="8"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="10"/>
       <c r="F25" s="6"/>
     </row>
@@ -2491,7 +2387,7 @@
       <c r="A26" s="5"/>
       <c r="B26" s="6"/>
       <c r="C26" s="10"/>
-      <c r="D26" s="11"/>
+      <c r="D26" s="44"/>
       <c r="E26" s="10"/>
       <c r="F26" s="6"/>
     </row>
@@ -2499,15 +2395,81 @@
       <c r="A27" s="5"/>
       <c r="B27" s="12"/>
       <c r="C27" s="13"/>
-      <c r="D27" s="11"/>
+      <c r="D27" s="44"/>
       <c r="E27" s="10"/>
       <c r="F27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="D28" s="11"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="10"/>
       <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="15"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D32" s="15"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="15"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="15"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="15"/>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="15"/>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="15"/>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="15"/>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="15"/>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D41" s="15"/>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D42" s="15"/>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D43" s="15"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D44" s="15"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D45" s="15"/>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="15"/>
+    </row>
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D47" s="15"/>
+    </row>
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D48" s="15"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D49" s="15"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2521,7 +2483,7 @@
   <sheetPr codeName="Rooms"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E50"/>
     </sheetView>
   </sheetViews>
@@ -2569,7 +2531,7 @@
         <v>880881</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -2584,7 +2546,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E3" s="24"/>
       <c r="F3" s="6"/>
@@ -2598,7 +2560,7 @@
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E4" s="24"/>
       <c r="F4" s="6"/>
@@ -2612,7 +2574,7 @@
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="6"/>
@@ -2660,7 +2622,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="6"/>
@@ -2676,7 +2638,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="6"/>
@@ -2692,7 +2654,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="6"/>
@@ -2806,7 +2768,7 @@
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="6"/>
@@ -2820,7 +2782,7 @@
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="6"/>
@@ -2834,7 +2796,7 @@
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="6"/>
@@ -2864,7 +2826,7 @@
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="6"/>
@@ -2923,7 +2885,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="F26" s="6"/>
     </row>
@@ -2949,7 +2911,7 @@
         <v>43</v>
       </c>
       <c r="D28" s="44" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="6"/>
@@ -2962,7 +2924,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E29" s="15"/>
     </row>

</xml_diff>

<commit_message>
add more rooms seems to be working
</commit_message>
<xml_diff>
--- a/spreadsheets/Communicator.xlsx
+++ b/spreadsheets/Communicator.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="90">
   <si>
     <t>Date Stamp</t>
   </si>
@@ -288,6 +288,21 @@
   </si>
   <si>
     <t>880,881</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -2192,34 +2207,66 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="5">
+        <v>43068</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="E2" s="23"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="5">
+        <v>43068</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>86</v>
+      </c>
       <c r="E3" s="24"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="5">
+        <v>43068</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="E4" s="24"/>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="5">
+        <v>43068</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>89</v>
+      </c>
       <c r="E5" s="24"/>
       <c r="F5" s="6"/>
     </row>

</xml_diff>